<commit_message>
add demo in ct
</commit_message>
<xml_diff>
--- a/Data/Lecanemab.xlsx
+++ b/Data/Lecanemab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Desktop\Master\P8105\Homework\Alzheimers_Disease_New_Hope\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CB19D8-79CD-4388-84D8-1916BB975AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D882DB3-E024-4190-8CE2-C0B54E6B4530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13251" yWindow="0" windowWidth="8778" windowHeight="11709" tabRatio="898" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11829" tabRatio="898" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="AE" sheetId="3" r:id="rId3"/>
     <sheet name="K-M" sheetId="4" r:id="rId4"/>
     <sheet name="safety" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="result" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -232,11 +232,11 @@
     <t>CDR-SB</t>
   </si>
   <si>
-    <t>ADAS-cog14</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>MMSE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ADAS-Cog14</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2539,7 +2539,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -2686,7 +2686,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -2742,7 +2742,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -2771,7 +2771,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -2815,7 +2815,7 @@
         <v>859</v>
       </c>
       <c r="F12">
-        <f t="shared" ref="F12:F15" si="2">C12-1.96*D12/SQRT(E12)</f>
+        <f t="shared" ref="F12:F14" si="2">C12-1.96*D12/SQRT(E12)</f>
         <v>40.758629375762887</v>
       </c>
       <c r="G12">
@@ -2914,7 +2914,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
@@ -2942,7 +2942,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>

</xml_diff>